<commit_message>
Fix validation after new fixes
</commit_message>
<xml_diff>
--- a/examples/columngrouplist.xlsx
+++ b/examples/columngrouplist.xlsx
@@ -82,12 +82,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
       <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
       <diagonal style="none"/>
     </border>
   </borders>
@@ -101,32 +116,28 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="0">
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
@@ -649,42 +660,42 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1"/>
@@ -705,96 +716,96 @@
         <v>7</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3" t="s">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="3"/>
+      <c r="N3" s="2"/>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" ht="17.399999999999999" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>45940</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>0.41666666666666702</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>45945</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>0.45833333333333298</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>45975</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>0.54166666666666696</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>45977</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="6">
         <v>0.58333333333333304</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>46005</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
         <v>0.625</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>46007</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="6">
         <v>0.70833333333333304</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix multiple attribute annotations
</commit_message>
<xml_diff>
--- a/examples/columngrouplist.xlsx
+++ b/examples/columngrouplist.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>Hamidov</t>
+  </si>
+  <si>
+    <t>Tashulya</t>
+  </si>
+  <si>
+    <t>Hamidova</t>
   </si>
 </sst>
 </file>
@@ -116,7 +122,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -138,6 +144,9 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="1" numFmtId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
@@ -809,6 +818,94 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7">
+        <v>45940</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E6" s="7">
+        <v>45945</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="G6" s="7">
+        <v>45975</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I6" s="7">
+        <v>45977</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="K6" s="7">
+        <v>46005</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="M6" s="7">
+        <v>46007</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7">
+        <v>45940</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E7" s="7">
+        <v>45945</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="G7" s="7">
+        <v>45975</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I7" s="7">
+        <v>45977</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="K7" s="7">
+        <v>46005</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="M7" s="7">
+        <v>46007</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A1:A4"/>

</xml_diff>

<commit_message>
Refactor - rename some classes
</commit_message>
<xml_diff>
--- a/examples/columngrouplist.xlsx
+++ b/examples/columngrouplist.xlsx
@@ -1,43 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr date1904="0"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0" showHorizontalScroll="1" showVerticalScroll="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
-  <si>
-    <t xml:space="preserve">Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Name</t>
   </si>
   <si>
     <t xml:space="preserve">Last name</t>
   </si>
   <si>
-    <t xml:space="preserve">Months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December</t>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
   </si>
   <si>
     <t xml:space="preserve">Day 1</t>
@@ -46,61 +43,41 @@
     <t xml:space="preserve">Day 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mansur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hamidov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tashulya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hamidova</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Mansur</t>
+  </si>
+  <si>
+    <t>Hamidov</t>
+  </si>
+  <si>
+    <t>Tashulya</t>
+  </si>
+  <si>
+    <t>Hamidova</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="h:mm"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.000000"/>
       <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,14 +89,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color theme="1"/>
       </left>
@@ -132,125 +109,395 @@
       <bottom style="thin">
         <color theme="1"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="6">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
+      <protection hidden="0" locked="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="1">
+      <protection hidden="0" locked="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="0" locked="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="New Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme>
+    <a:fmtScheme name="">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -277,7 +524,6 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -301,7 +547,6 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -320,13 +565,31 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -361,38 +624,38 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr filterMode="0">
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5:L5"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" zoomScale="100" workbookViewId="0">
+      <selection activeCell="K5" activeCellId="0" sqref="K5:L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.28"/>
+    <col customWidth="1" min="3" max="3" style="1" width="10.539999999999999"/>
+    <col customWidth="1" min="5" max="5" style="1" width="10.539999999999999"/>
+    <col customWidth="1" min="7" max="7" style="1" width="10.539999999999999"/>
+    <col customWidth="1" min="9" max="9" style="1" width="10.539999999999999"/>
+    <col customWidth="1" min="11" max="11" style="1" width="13"/>
+    <col customWidth="1" min="12" max="12" style="1" width="14.279999999999999"/>
+    <col customWidth="1" min="13" max="13" style="1" width="12"/>
+    <col customWidth="1" min="14" max="14" style="1" width="12.279999999999999"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" ht="14.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -414,7 +677,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" ht="14.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -436,7 +699,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" ht="14.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -464,7 +727,7 @@
       </c>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" ht="14.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
@@ -504,125 +767,123 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" ht="17.399999999999999" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="4">
         <v>45940</v>
       </c>
-      <c r="D5" s="5" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="E5" s="4" t="n">
+      <c r="D5" s="5">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E5" s="4">
         <v>45945</v>
       </c>
-      <c r="F5" s="5" t="n">
-        <v>0.458333333333333</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4" t="n">
+      <c r="F5" s="5">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="G5" s="4">
         <v>45977</v>
       </c>
-      <c r="J5" s="5" t="n">
-        <v>0.583333333333333</v>
-      </c>
-      <c r="K5" s="4" t="n">
+      <c r="H5" s="5">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="K5" s="4">
         <v>46005</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="5">
         <v>0.625</v>
       </c>
-      <c r="M5" s="4" t="n">
+      <c r="M5" s="4">
         <v>46007</v>
       </c>
-      <c r="N5" s="5" t="n">
-        <v>0.708333333333333</v>
+      <c r="N5" s="5">
+        <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="4">
         <v>45940</v>
       </c>
-      <c r="D6" s="5" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="E6" s="4" t="n">
+      <c r="D6" s="5">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E6" s="4">
         <v>45945</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="5">
         <v>0.375</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="4">
         <v>45975</v>
       </c>
-      <c r="H6" s="5" t="n">
-        <v>0.583333333333333</v>
-      </c>
-      <c r="I6" s="4" t="n">
+      <c r="H6" s="5">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="I6" s="4">
         <v>45977</v>
       </c>
-      <c r="J6" s="5" t="n">
-        <v>0.583333333333333</v>
-      </c>
-      <c r="K6" s="4" t="n">
+      <c r="J6" s="5">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="K6" s="4">
         <v>46005</v>
       </c>
-      <c r="L6" s="5" t="n">
+      <c r="L6" s="5">
         <v>0.625</v>
       </c>
-      <c r="M6" s="4" t="n">
+      <c r="M6" s="4">
         <v>46007</v>
       </c>
-      <c r="N6" s="5" t="n">
-        <v>0.708333333333333</v>
+      <c r="N6" s="5">
+        <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="4">
         <v>45940</v>
       </c>
-      <c r="D7" s="5" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="E7" s="4" t="n">
+      <c r="D7" s="5">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E7" s="4">
         <v>45945</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="5">
         <v>0.375</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="4">
         <v>45975</v>
       </c>
-      <c r="H7" s="5" t="n">
-        <v>0.583333333333333</v>
-      </c>
-      <c r="I7" s="4" t="n">
+      <c r="H7" s="5">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="I7" s="4">
         <v>45977</v>
       </c>
-      <c r="J7" s="5" t="n">
-        <v>0.583333333333333</v>
-      </c>
-      <c r="K7" s="4" t="n">
+      <c r="J7" s="5">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="K7" s="4">
         <v>46005</v>
       </c>
-      <c r="L7" s="5" t="n">
+      <c r="L7" s="5">
         <v>0.625</v>
       </c>
       <c r="M7" s="4"/>
@@ -643,12 +904,9 @@
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <printOptions headings="0" gridLines="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51181102362204689" footer="0.51181102362204689"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>